<commit_message>
Revision antes de 3ra produccion SETI
Se actuliza la columna NEW
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/04.PRODUCCION/SETI-BATCH-2_MAY2023/02-BOM/BATT_CONNECTOR.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/04.PRODUCCION/SETI-BATCH-2_MAY2023/02-BOM/BATT_CONNECTOR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER-1K/02.BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER R-1/04.PRODUCCION/SETI-BATCH-2_MAY2023/02-BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86021842-7470-234A-9076-3FA13901FE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695E09C6-A30F-9945-B536-0A002C6E6160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Qty</t>
   </si>
@@ -88,9 +88,6 @@
     <t>NEW</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Transistor</t>
   </si>
   <si>
@@ -173,6 +170,12 @@
   </si>
   <si>
     <t>VERSION</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Se actualiza columna NEW para 3ra produccion de SETI</t>
   </si>
 </sst>
 </file>
@@ -864,7 +867,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -905,6 +908,10 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -917,10 +924,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1377,7 +1381,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1398,12 +1402,12 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="22">
+      <c r="B2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="18">
         <f>MAX(_HISTORY!A4:A42)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
@@ -1413,12 +1417,12 @@
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
@@ -1457,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1466,16 +1470,16 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
         <v>40</v>
       </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>41</v>
-      </c>
       <c r="H7" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1483,7 +1487,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1495,7 +1499,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>13</v>
@@ -1506,7 +1510,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1518,10 +1522,10 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>14</v>
@@ -1555,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F394E835-0523-104C-AA22-72C38CD42C08}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1568,21 +1572,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1593,10 +1597,10 @@
         <v>44874</v>
       </c>
       <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
         <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1607,10 +1611,10 @@
         <v>44880</v>
       </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1618,13 +1622,27 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="24">
+        <v>45195</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1643,22 +1661,22 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="A1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
@@ -1672,14 +1690,14 @@
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -1691,19 +1709,19 @@
     </row>
     <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="C9" s="12"/>
     </row>

</xml_diff>